<commit_message>
Aggiornamento ultimi risultati sperimentazione & ultimi fix - Inoltre, README.md aggiornato
Signed-off-by: Gianmarco Scarano <gianmarcoscarano@gmail.com>
</commit_message>
<xml_diff>
--- a/Results/Risultati.xlsx
+++ b/Results/Risultati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Università\Sistemi ad Agenti\Progetto\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5117EC27-807D-4C7A-84F2-05D4C1E201F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB75BD5-D000-4179-AC31-EEFFAC0EFFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="42">
   <si>
     <t>BATCH</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>In corso</t>
   </si>
   <si>
     <t>Models/Gruppo_G</t>
@@ -130,10 +127,31 @@
     <t>Models/Gruppo_I</t>
   </si>
   <si>
-    <t>Programmato</t>
-  </si>
-  <si>
     <t>DemosEmovo</t>
+  </si>
+  <si>
+    <t>Models/Gruppo_K</t>
+  </si>
+  <si>
+    <t>Models/Gruppo_J</t>
+  </si>
+  <si>
+    <t>Models/Gruppo_L</t>
+  </si>
+  <si>
+    <t>Models/Gruppo_M</t>
+  </si>
+  <si>
+    <t>Models/Gruppo_N</t>
+  </si>
+  <si>
+    <t>Models/Gruppo_O</t>
+  </si>
+  <si>
+    <t>DemosEmovoGender</t>
+  </si>
+  <si>
+    <t>Models/Gruppo_P</t>
   </si>
 </sst>
 </file>
@@ -556,12 +574,12 @@
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.5703125" bestFit="1" customWidth="1"/>
@@ -621,7 +639,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -646,14 +664,22 @@
       <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="I2" s="9">
+        <v>3.1921499999999999E-3</v>
+      </c>
+      <c r="J2" s="9">
+        <v>0.90293546999999996</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0.99850000000000005</v>
+      </c>
+      <c r="L2" s="7">
+        <v>0.80842999999999998</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -680,14 +706,22 @@
       <c r="H3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6" t="s">
+      <c r="I3" s="9">
+        <v>5.1311400000000002E-3</v>
+      </c>
+      <c r="J3" s="9">
+        <v>2.8856434399999999</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0.99829999999999997</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0.53576999999999997</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14" ht="39" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -700,7 +734,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="6">
         <v>64</v>
@@ -714,16 +748,22 @@
       <c r="H4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
+      <c r="I4" s="9">
+        <v>1.5443200000000001E-3</v>
+      </c>
+      <c r="J4" s="9">
+        <v>1.90271166</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0.99929000000000001</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0.71970999999999996</v>
+      </c>
       <c r="M4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -778,7 +818,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="6">
         <v>64</v>
@@ -792,20 +832,26 @@
       <c r="H6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
+      <c r="I6" s="9">
+        <v>1.3681100000000001E-3</v>
+      </c>
+      <c r="J6" s="9">
+        <v>1.0328782400000001</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0.99961</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0.84060999999999997</v>
+      </c>
       <c r="M6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N6" s="6" t="s">
         <v>29</v>
       </c>
+      <c r="N6" s="6"/>
     </row>
     <row r="7" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>19</v>
@@ -817,7 +863,7 @@
         <v>28</v>
       </c>
       <c r="E7" s="6">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="F7" s="6">
         <v>100</v>
@@ -828,18 +874,26 @@
       <c r="H7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="I7" s="9">
+        <v>2.53587E-3</v>
+      </c>
+      <c r="J7" s="9">
+        <v>1.5058463600000001</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0.99843999999999999</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0.76334000000000002</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>23</v>
@@ -862,18 +916,26 @@
       <c r="H8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="I8" s="9">
+        <v>7.7734800000000001E-3</v>
+      </c>
+      <c r="J8" s="9">
+        <v>2.7870627799999999</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0.99804000000000004</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0.50702000000000003</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>12</v>
@@ -896,18 +958,26 @@
       <c r="H9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="9">
+        <v>4.9635E-3</v>
+      </c>
+      <c r="J9" s="9">
+        <v>1.0978026599999999</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0.99887999999999999</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0.73387999999999998</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N9" s="6"/>
+    </row>
+    <row r="10" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>19</v>
@@ -922,7 +992,7 @@
         <v>64</v>
       </c>
       <c r="F10" s="6">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>14</v>
@@ -931,25 +1001,25 @@
         <v>15</v>
       </c>
       <c r="I10" s="9">
-        <v>1.09370368</v>
+        <v>7.2946599999999997E-3</v>
       </c>
       <c r="J10" s="9">
-        <v>1.9895078799999999</v>
+        <v>7.1528560000000005E-2</v>
       </c>
       <c r="K10" s="7">
-        <v>0.60799000000000003</v>
+        <v>0.99773000000000001</v>
       </c>
       <c r="L10" s="7">
-        <v>0.39795999999999998</v>
+        <v>0.9778</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="N10" s="6"/>
     </row>
     <row r="11" spans="1:14" ht="39" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>19</v>
@@ -958,13 +1028,13 @@
         <v>13</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="6">
         <v>64</v>
       </c>
       <c r="F11" s="6">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>14</v>
@@ -973,28 +1043,28 @@
         <v>15</v>
       </c>
       <c r="I11" s="9">
-        <v>1.33692031</v>
+        <v>6.4497659999999998E-2</v>
       </c>
       <c r="J11" s="9">
-        <v>1.66391975</v>
+        <v>7.9061080000000006E-2</v>
       </c>
       <c r="K11" s="7">
-        <v>0.46938999999999997</v>
+        <v>0.97599000000000002</v>
       </c>
       <c r="L11" s="7">
-        <v>0.35204000000000002</v>
+        <v>0.97119</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="N11" s="6"/>
     </row>
-    <row r="12" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>13</v>
@@ -1015,19 +1085,19 @@
         <v>15</v>
       </c>
       <c r="I12" s="9">
-        <v>0.66171325999999997</v>
+        <v>1.09370368</v>
       </c>
       <c r="J12" s="9">
-        <v>2.0823479300000001</v>
+        <v>1.9895078799999999</v>
       </c>
       <c r="K12" s="7">
-        <v>0.85204000000000002</v>
+        <v>0.60799000000000003</v>
       </c>
       <c r="L12" s="7">
-        <v>0.34694000000000003</v>
+        <v>0.39795999999999998</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="N12" s="6"/>
     </row>
@@ -1036,13 +1106,13 @@
         <v>18</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="6">
         <v>64</v>
@@ -1057,19 +1127,19 @@
         <v>15</v>
       </c>
       <c r="I13" s="9">
-        <v>1.6925559999999999E-2</v>
+        <v>1.33692031</v>
       </c>
       <c r="J13" s="9">
-        <v>3.0186173900000002</v>
+        <v>1.66391975</v>
       </c>
       <c r="K13" s="7">
-        <v>1</v>
+        <v>0.46938999999999997</v>
       </c>
       <c r="L13" s="7">
-        <v>0.51019999999999999</v>
+        <v>0.35204000000000002</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N13" s="6"/>
     </row>
@@ -1078,7 +1148,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>13</v>
@@ -1099,19 +1169,19 @@
         <v>15</v>
       </c>
       <c r="I14" s="9">
-        <v>0.66143768999999997</v>
+        <v>0.66171325999999997</v>
       </c>
       <c r="J14" s="9">
-        <v>2.0486019299999998</v>
+        <v>2.0823479300000001</v>
       </c>
       <c r="K14" s="7">
-        <v>0.72448999999999997</v>
+        <v>0.85204000000000002</v>
       </c>
       <c r="L14" s="7">
-        <v>0.36735000000000001</v>
+        <v>0.34694000000000003</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N14" s="6"/>
     </row>
@@ -1120,13 +1190,13 @@
         <v>18</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="6">
         <v>64</v>
@@ -1141,52 +1211,104 @@
         <v>15</v>
       </c>
       <c r="I15" s="9">
+        <v>1.6925559999999999E-2</v>
+      </c>
+      <c r="J15" s="9">
+        <v>3.0186173900000002</v>
+      </c>
+      <c r="K15" s="7">
+        <v>1</v>
+      </c>
+      <c r="L15" s="7">
+        <v>0.51019999999999999</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="6">
+        <v>64</v>
+      </c>
+      <c r="F16" s="6">
+        <v>100</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="9">
+        <v>0.66143768999999997</v>
+      </c>
+      <c r="J16" s="9">
+        <v>2.0486019299999998</v>
+      </c>
+      <c r="K16" s="7">
+        <v>0.72448999999999997</v>
+      </c>
+      <c r="L16" s="7">
+        <v>0.36735000000000001</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="1:14" ht="39" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="6">
+        <v>64</v>
+      </c>
+      <c r="F17" s="6">
+        <v>100</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="9">
         <v>1.80430844</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J17" s="9">
         <v>3.14981008</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K17" s="7">
         <v>0.29082000000000002</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L17" s="7">
         <v>0.28571000000000002</v>
       </c>
-      <c r="M15" s="6" t="s">
+      <c r="M17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="6"/>
-    </row>
-    <row r="16" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-    </row>
-    <row r="17" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="6"/>
       <c r="N17" s="6"/>
     </row>
     <row r="18" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
@@ -1622,12 +1744,12 @@
       <c r="N44" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N15">
-    <sortCondition ref="A2:A15"/>
-    <sortCondition ref="B2:B15"/>
-    <sortCondition ref="C2:C15"/>
-    <sortCondition ref="D2:D15"/>
-    <sortCondition ref="M2:M15"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N17">
+    <sortCondition ref="A2:A17"/>
+    <sortCondition ref="B2:B17"/>
+    <sortCondition ref="C2:C17"/>
+    <sortCondition ref="D2:D17"/>
+    <sortCondition ref="M2:M17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Validation phase, nuovo dataset e fixes per script di training - Incluso nuovo dataset "Opera7" nello script di download - Incluso nuovo dataset "Opera7" nello script dei CSV - Aggiunti parametri per utilizzare Drive / Mega e Augmentation per lo script di download dei dataset - Aggiunto parametro "loadModel" per caricare un modello per fare validation - Aggiunto parametro "validation" per decidere se fare validation su "gender" o "emotion" - Incluso nuovo dataLoader "Opera7" - Più scalabilità tra i vari dataLoader - Fix numero di classi nello script di Train - Nuovi parametri per i checkpoint ("val_correct" / "val_samples") - Creazione script di validation con creazione di report di classificazione e confusion matrix - Importazione metodi di Confusion Matrix - Update README.md - Update .gitignore
Signed-off-by: Gianmarco Scarano <gianmarcoscarano@gmail.com>
</commit_message>
<xml_diff>
--- a/Results/Risultati.xlsx
+++ b/Results/Risultati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Università\Sistemi ad Agenti\Progetto\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB75BD5-D000-4179-AC31-EEFFAC0EFFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2DE761-9B0A-4176-8C03-4FA069F2706D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,7 +162,7 @@
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,13 +198,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Lato"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Lato"/>
@@ -252,7 +245,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -285,9 +278,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -571,28 +561,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.85546875" customWidth="1"/>
-    <col min="14" max="14" width="37.5703125" customWidth="1"/>
+    <col min="13" max="13" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1001,16 +991,16 @@
         <v>15</v>
       </c>
       <c r="I10" s="9">
-        <v>7.2946599999999997E-3</v>
+        <v>9.6511199999999991E-3</v>
       </c>
       <c r="J10" s="9">
-        <v>7.1528560000000005E-2</v>
+        <v>9.3743090000000001E-2</v>
       </c>
       <c r="K10" s="7">
-        <v>0.99773000000000001</v>
+        <v>0.99573999999999996</v>
       </c>
       <c r="L10" s="7">
-        <v>0.9778</v>
+        <v>0.97638000000000003</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>39</v>
@@ -1042,17 +1032,17 @@
       <c r="H11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="9">
-        <v>6.4497659999999998E-2</v>
+      <c r="I11" s="6">
+        <v>9.6259120000000004E-2</v>
       </c>
       <c r="J11" s="9">
-        <v>7.9061080000000006E-2</v>
+        <v>9.7210359999999996E-2</v>
       </c>
       <c r="K11" s="7">
-        <v>0.97599000000000002</v>
+        <v>0.96570999999999996</v>
       </c>
       <c r="L11" s="7">
-        <v>0.97119</v>
+        <v>0.96221000000000001</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>41</v>
@@ -1312,29 +1302,15 @@
       <c r="N17" s="6"/>
     </row>
     <row r="18" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="12"/>
+      <c r="N18" s="6"/>
     </row>
     <row r="19" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
@@ -1344,13 +1320,6 @@
       <c r="N19" s="6"/>
     </row>
     <row r="20" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
@@ -1360,13 +1329,6 @@
       <c r="N20" s="6"/>
     </row>
     <row r="21" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
@@ -1376,13 +1338,6 @@
       <c r="N21" s="6"/>
     </row>
     <row r="22" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -1392,13 +1347,6 @@
       <c r="N22" s="6"/>
     </row>
     <row r="23" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -1408,13 +1356,6 @@
       <c r="N23" s="6"/>
     </row>
     <row r="24" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
@@ -1423,149 +1364,149 @@
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
     </row>
-    <row r="25" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-    </row>
-    <row r="26" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
+    <row r="25" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
     </row>
     <row r="28" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
     </row>
     <row r="31" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-    </row>
-    <row r="32" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+    </row>
+    <row r="32" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+    </row>
+    <row r="33" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
     </row>
     <row r="34" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
@@ -1576,10 +1517,10 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
     </row>
@@ -1593,9 +1534,9 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
     </row>
@@ -1609,9 +1550,9 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
     </row>
@@ -1625,123 +1566,11 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
-    </row>
-    <row r="38" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-    </row>
-    <row r="39" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-    </row>
-    <row r="40" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-    </row>
-    <row r="41" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-    </row>
-    <row r="42" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-    </row>
-    <row r="43" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-    </row>
-    <row r="44" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N17">

</xml_diff>

<commit_message>
Aggiunta validation con Vokaturi e aggiornamento risultati - Aggiunto script per generare risultati tramite Vokaturi - Fix per cache di CUDA
Signed-off-by: Gianmarco Scarano <gianmarcoscarano@gmail.com>
</commit_message>
<xml_diff>
--- a/Results/Risultati.xlsx
+++ b/Results/Risultati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Università\Sistemi ad Agenti\Progetto\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2DE761-9B0A-4176-8C03-4FA069F2706D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339C90E9-751C-4202-897B-2C775F04D557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3945" windowWidth="24585" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="42">
-  <si>
-    <t>BATCH</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="47">
   <si>
     <t>ATTENTION</t>
   </si>
@@ -152,6 +149,25 @@
   </si>
   <si>
     <t>Models/Gruppo_P</t>
+  </si>
+  <si>
+    <t>Validation corretta su Colab.</t>
+  </si>
+  <si>
+    <t>Validation corretta 
+su Server Cilab.</t>
+  </si>
+  <si>
+    <t>Validation corretta in locale.</t>
+  </si>
+  <si>
+    <t>VALIDATION</t>
+  </si>
+  <si>
+    <t>Emotion</t>
+  </si>
+  <si>
+    <t>Gender</t>
   </si>
 </sst>
 </file>
@@ -162,7 +178,7 @@
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +214,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Lato"/>
@@ -245,7 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -278,6 +301,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -561,98 +587,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
+    <col min="13" max="13" width="27.85546875" customWidth="1"/>
+    <col min="14" max="14" width="56.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="M1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="6">
-        <v>64</v>
+        <v>27</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F2" s="6">
         <v>100</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="I2" s="9">
         <v>3.1921499999999999E-3</v>
@@ -667,34 +693,36 @@
         <v>0.80842999999999998</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="N2" s="6"/>
+        <v>37</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="6">
-        <v>64</v>
+        <v>27</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F3" s="6">
         <v>100</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="I3" s="9">
         <v>5.1311400000000002E-3</v>
@@ -709,118 +737,124 @@
         <v>0.53576999999999997</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="1:14" ht="39" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="6">
-        <v>64</v>
+        <v>29</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F4" s="6">
         <v>100</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="I4" s="9">
-        <v>1.5443200000000001E-3</v>
+        <v>2.9442299999999999E-3</v>
       </c>
       <c r="J4" s="9">
-        <v>1.90271166</v>
+        <v>1.81546082</v>
       </c>
       <c r="K4" s="7">
-        <v>0.99929000000000001</v>
+        <v>0.99873000000000001</v>
       </c>
       <c r="L4" s="7">
-        <v>0.71970999999999996</v>
+        <v>0.71240999999999999</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="6">
-        <v>42</v>
+        <v>27</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F5" s="6">
         <v>100</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="I5" s="9">
-        <v>1.6254500000000001E-3</v>
+        <v>1.4042E-3</v>
       </c>
       <c r="J5" s="9">
-        <v>0.55719748000000002</v>
+        <v>1.42221274</v>
       </c>
       <c r="K5" s="7">
-        <v>0.99955000000000005</v>
+        <v>0.99929999999999997</v>
       </c>
       <c r="L5" s="7">
-        <v>0.88114000000000003</v>
+        <v>0.73624999999999996</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="39" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="D6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="6">
-        <v>64</v>
+        <v>29</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F6" s="6">
         <v>100</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="I6" s="9">
         <v>1.3681100000000001E-3</v>
@@ -835,34 +869,36 @@
         <v>0.84060999999999997</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="6"/>
-    </row>
-    <row r="7" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="6">
-        <v>42</v>
+        <v>27</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F7" s="6">
         <v>100</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="I7" s="9">
         <v>2.53587E-3</v>
@@ -877,34 +913,36 @@
         <v>0.76334000000000002</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N7" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="6">
-        <v>64</v>
+        <v>27</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F8" s="6">
         <v>100</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="I8" s="9">
         <v>7.7734800000000001E-3</v>
@@ -919,34 +957,36 @@
         <v>0.50702000000000003</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="6">
-        <v>64</v>
+        <v>27</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F9" s="6">
         <v>100</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="I9" s="9">
         <v>4.9635E-3</v>
@@ -961,118 +1001,124 @@
         <v>0.73387999999999998</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="N9" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="6">
-        <v>64</v>
+        <v>27</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="F10" s="6">
         <v>10</v>
       </c>
       <c r="G10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="I10" s="9">
-        <v>9.6511199999999991E-3</v>
+        <v>1.8842790000000002E-2</v>
       </c>
       <c r="J10" s="9">
-        <v>9.3743090000000001E-2</v>
+        <v>6.6671069999999999E-2</v>
       </c>
       <c r="K10" s="7">
-        <v>0.99573999999999996</v>
+        <v>0.99260999999999999</v>
       </c>
       <c r="L10" s="7">
-        <v>0.97638000000000003</v>
+        <v>0.9778</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="N10" s="6"/>
+        <v>38</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="39" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="6">
-        <v>64</v>
+        <v>29</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="F11" s="6">
         <v>10</v>
       </c>
       <c r="G11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="I11" s="6">
-        <v>9.6259120000000004E-2</v>
+        <v>8.0490820000000005E-2</v>
       </c>
       <c r="J11" s="9">
-        <v>9.7210359999999996E-2</v>
+        <v>0.1024118</v>
       </c>
       <c r="K11" s="7">
-        <v>0.96570999999999996</v>
+        <v>0.97082999999999997</v>
       </c>
       <c r="L11" s="7">
-        <v>0.96221000000000001</v>
+        <v>0.96267999999999998</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="N11" s="6"/>
+        <v>40</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="C12" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="6">
-        <v>64</v>
+        <v>27</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F12" s="6">
         <v>100</v>
       </c>
       <c r="G12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="I12" s="9">
         <v>1.09370368</v>
@@ -1087,34 +1133,36 @@
         <v>0.39795999999999998</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N12" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" spans="1:14" ht="39" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="C13" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="6">
-        <v>64</v>
+        <v>29</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F13" s="6">
         <v>100</v>
       </c>
       <c r="G13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="I13" s="9">
         <v>1.33692031</v>
@@ -1129,34 +1177,36 @@
         <v>0.35204000000000002</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="14" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="6">
-        <v>64</v>
+        <v>27</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F14" s="6">
         <v>100</v>
       </c>
       <c r="G14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="I14" s="9">
         <v>0.66171325999999997</v>
@@ -1171,34 +1221,36 @@
         <v>0.34694000000000003</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="N14" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" spans="1:14" ht="39" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="6">
-        <v>64</v>
+        <v>29</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F15" s="6">
         <v>100</v>
       </c>
       <c r="G15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="I15" s="9">
         <v>1.6925559999999999E-2</v>
@@ -1213,34 +1265,36 @@
         <v>0.51019999999999999</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N15" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="16" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="D16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="6">
-        <v>64</v>
+        <v>27</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F16" s="6">
         <v>100</v>
       </c>
       <c r="G16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="I16" s="9">
         <v>0.66143768999999997</v>
@@ -1255,34 +1309,36 @@
         <v>0.36735000000000001</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N16" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="17" spans="1:14" ht="39" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="D17" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="6">
-        <v>64</v>
+        <v>29</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F17" s="6">
         <v>100</v>
       </c>
       <c r="G17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="I17" s="9">
         <v>1.80430844</v>
@@ -1297,20 +1353,34 @@
         <v>0.28571000000000002</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N17" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="18" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
+      <c r="N18" s="12"/>
     </row>
     <row r="19" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
@@ -1320,6 +1390,12 @@
       <c r="N19" s="6"/>
     </row>
     <row r="20" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
@@ -1329,6 +1405,12 @@
       <c r="N20" s="6"/>
     </row>
     <row r="21" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
@@ -1338,6 +1420,12 @@
       <c r="N21" s="6"/>
     </row>
     <row r="22" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -1347,6 +1435,12 @@
       <c r="N22" s="6"/>
     </row>
     <row r="23" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -1356,6 +1450,12 @@
       <c r="N23" s="6"/>
     </row>
     <row r="24" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
@@ -1364,149 +1464,149 @@
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
     </row>
-    <row r="25" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+    <row r="25" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+    </row>
+    <row r="26" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
     </row>
     <row r="27" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
     </row>
     <row r="28" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
     </row>
     <row r="29" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
     </row>
     <row r="30" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
     </row>
     <row r="31" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
     </row>
     <row r="32" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
     </row>
     <row r="33" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
     </row>
     <row r="34" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
@@ -1517,10 +1617,10 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
     </row>
@@ -1534,9 +1634,9 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
     </row>
@@ -1550,9 +1650,9 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
     </row>
@@ -1566,19 +1666,123 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
+    </row>
+    <row r="38" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+    </row>
+    <row r="39" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+    </row>
+    <row r="40" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+    </row>
+    <row r="41" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+    </row>
+    <row r="42" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+    </row>
+    <row r="43" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+    </row>
+    <row r="44" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N17">
     <sortCondition ref="A2:A17"/>
     <sortCondition ref="B2:B17"/>
-    <sortCondition ref="C2:C17"/>
     <sortCondition ref="D2:D17"/>
-    <sortCondition ref="M2:M17"/>
+    <sortCondition ref="L2:L17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>